<commit_message>
Kanban_Board formating code cal 20
</commit_message>
<xml_diff>
--- a/formating_code/Kanban_cal/Kanban_Board.xlsx
+++ b/formating_code/Kanban_cal/Kanban_Board.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24E6227-15C2-447E-A586-EFE31F77BC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F3778E-47A2-4D2E-A141-EECBF76C0C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3225" yWindow="3690" windowWidth="21600" windowHeight="11505" tabRatio="788" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>Примечания</t>
   </si>
@@ -101,7 +101,10 @@
     <t>воскресенье</t>
   </si>
   <si>
-    <t>formatting the code ..</t>
+    <t xml:space="preserve">formatting the code .. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revise math … vidio 2 </t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;lei&quot;_-;\-* #,##0.00\ &quot;lei&quot;_-;_-* &quot;-&quot;??\ &quot;lei&quot;_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0\ &quot;lei&quot;_-;\-* #,##0\ &quot;lei&quot;_-;_-* &quot;-&quot;\ &quot;lei&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -342,6 +345,14 @@
       <color rgb="FFC00000"/>
       <name val="Century Gothic"/>
       <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1060,7 +1071,7 @@
     <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1187,6 +1198,9 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="14" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1250,7 +1264,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="11" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="27" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -2293,7 +2307,7 @@
   </sheetPr>
   <dimension ref="B1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -2315,12 +2329,12 @@
       </c>
     </row>
     <row r="2" spans="2:12" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="str">
+      <c r="B2" s="43" t="str">
         <f>"Январь "&amp;ГодКалендаря</f>
         <v>Январь 2023</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2355,10 +2369,10 @@
         <f t="shared" si="0"/>
         <v>суббота</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="2:12" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="29">
@@ -2545,22 +2559,22 @@
       <c r="C14" s="31">
         <v>44963</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
     </row>
     <row r="15" spans="2:12" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2635,12 +2649,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="str">
+      <c r="B2" s="59" t="str">
         <f>"Октябрь "&amp;ГодКалендаря</f>
         <v>Октябрь 2023</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2849,22 +2863,22 @@
       <c r="C14" s="34">
         <v>45236</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2926,12 +2940,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="str">
+      <c r="B2" s="59" t="str">
         <f>"Ноябрь "&amp;ГодКалендаря</f>
         <v>Ноябрь 2023</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3140,22 +3154,22 @@
       <c r="C14" s="34">
         <v>45264</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3217,12 +3231,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="str">
+      <c r="B2" s="43" t="str">
         <f>"Декабрь "&amp;ГодКалендаря</f>
         <v>Декабрь 2023</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3431,22 +3445,22 @@
       <c r="C14" s="31">
         <v>45292</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3508,12 +3522,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="str">
+      <c r="B2" s="43" t="str">
         <f>"Февраль "&amp;ГодКалендаря</f>
         <v>Февраль 2023</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3722,22 +3736,22 @@
       <c r="C14" s="31">
         <v>44991</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3799,12 +3813,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="str">
+      <c r="B2" s="49" t="str">
         <f>"Март "&amp;ГодКалендаря</f>
         <v>Март 2023</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4013,22 +4027,22 @@
       <c r="C14" s="40">
         <v>45019</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4090,12 +4104,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="str">
+      <c r="B2" s="49" t="str">
         <f>"Апрель "&amp;ГодКалендаря</f>
         <v>Апрель 2023</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4304,22 +4318,22 @@
       <c r="C14" s="40">
         <v>45047</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4381,12 +4395,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="str">
+      <c r="B2" s="49" t="str">
         <f>"Май "&amp;ГодКалендаря</f>
         <v>Май 2023</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4595,22 +4609,22 @@
       <c r="C14" s="40">
         <v>45082</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4672,12 +4686,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="str">
+      <c r="B2" s="54" t="str">
         <f>"Июнь "&amp;ГодКалендаря</f>
         <v>Июнь 2023</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4886,22 +4900,22 @@
       <c r="C14" s="37">
         <v>45110</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4963,12 +4977,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="str">
+      <c r="B2" s="54" t="str">
         <f>"Июль "&amp;ГодКалендаря</f>
         <v>Июль 2023</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5177,22 +5191,22 @@
       <c r="C14" s="37">
         <v>45138</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5254,12 +5268,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="str">
+      <c r="B2" s="54" t="str">
         <f>"Август "&amp;ГодКалендаря</f>
         <v>Август 2023</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5468,22 +5482,22 @@
       <c r="C14" s="37">
         <v>45173</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5529,7 +5543,7 @@
   <dimension ref="B1:I15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -5547,12 +5561,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="str">
+      <c r="B2" s="59" t="str">
         <f>"Сентябрь "&amp;ГодКалендаря</f>
         <v>Сентябрь 2023</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5713,10 +5727,12 @@
     </row>
     <row r="11" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="64" t="s">
+        <v>7</v>
+      </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
@@ -5763,22 +5779,22 @@
       <c r="C14" s="34">
         <v>45201</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
     </row>
     <row r="15" spans="2:9" s="10" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5816,6 +5832,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="426e97fa315356fffbdcd9876fe988c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14b8f0def80e6d70ce3def20c90759ae" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -6036,25 +6070,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{160D437D-D97C-4174-9BD0-B6C4706C93C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF997A1-6F4D-40DF-902F-6A09A77F9752}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65DF88E0-C534-44A9-B15A-DDE8DD22045C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6071,22 +6105,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF997A1-6F4D-40DF-902F-6A09A77F9752}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{160D437D-D97C-4174-9BD0-B6C4706C93C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>